<commit_message>
Added LFS tracking for geo data.
</commit_message>
<xml_diff>
--- a/data/fppe_data_combined.xlsx
+++ b/data/fppe_data_combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshay/Workspace/MLC/FPPE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D6BBEC-10C3-4C4D-B23D-6829181E95F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D8B137-466A-DE4A-B964-DD91E3EAFB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{259E7114-D380-BD40-B813-EE9B97F880CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{259E7114-D380-BD40-B813-EE9B97F880CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>Combined</t>
   </si>
   <si>
-    <t>Andaman &amp; Nicobar Islands</t>
-  </si>
-  <si>
     <t>Andhra Pradesh</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>Delhi</t>
   </si>
   <si>
-    <t>Dadra &amp; Nagar Haveli and Daman &amp; Diu</t>
-  </si>
-  <si>
     <t>Goa</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Himachal Pradesh</t>
   </si>
   <si>
-    <t>Jammu &amp; Kashmir</t>
-  </si>
-  <si>
     <t>Jharkhand</t>
   </si>
   <si>
@@ -234,6 +225,15 @@
   </si>
   <si>
     <t>Haryana</t>
+  </si>
+  <si>
+    <t>Andaman &amp; Nicobar</t>
+  </si>
+  <si>
+    <t>Jammu and Kashmir</t>
+  </si>
+  <si>
+    <t>Dadra &amp; Nagar Haveli &amp; Daman &amp; Diu</t>
   </si>
 </sst>
 </file>
@@ -299,14 +299,14 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,193 +631,193 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+      <c r="AO1" s="4"/>
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4" t="s">
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4" t="s">
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4" t="s">
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="4" t="s">
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AQ2" s="4"/>
+      <c r="AQ2" s="5"/>
     </row>
     <row r="3" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5" t="s">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5" t="s">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5" t="s">
+      <c r="S3" s="3"/>
+      <c r="T3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5" t="s">
+      <c r="U3" s="3"/>
+      <c r="V3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5" t="s">
+      <c r="W3" s="3"/>
+      <c r="X3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5" t="s">
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5" t="s">
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5" t="s">
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5" t="s">
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5" t="s">
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5" t="s">
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5" t="s">
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="5" t="s">
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AO3" s="5"/>
-      <c r="AP3" s="5" t="s">
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AQ3" s="5"/>
+      <c r="AQ3" s="3"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -950,7 +950,7 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1">
         <v>53.5</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1">
         <v>50.8</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1">
         <v>69.5</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>31.7</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>52.4</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>24.1</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
         <v>74</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>57.7</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>54.9</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1">
         <v>36.200000000000003</v>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1">
         <v>26.3</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>46.9</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1">
         <v>63.7</v>
@@ -2653,7 +2653,7 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1">
         <v>57</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1">
         <v>57.1</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1">
         <v>40.4</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1">
         <v>51.8</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1">
         <v>53.1</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1">
         <v>66.599999999999994</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1">
         <v>29.7</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1">
         <v>51.4</v>
@@ -3699,7 +3699,7 @@
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B26" s="1">
         <v>64.8</v>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B27" s="1">
         <v>23.6</v>
@@ -3961,7 +3961,7 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B28" s="1">
         <v>24.3</v>
@@ -4092,7 +4092,7 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="1">
         <v>35.299999999999997</v>
@@ -4223,7 +4223,7 @@
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1">
         <v>26.5</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1">
         <v>57.3</v>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1">
         <v>61.9</v>
@@ -4616,7 +4616,7 @@
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1">
         <v>75.8</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1">
         <v>59.7</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B35" s="1">
         <v>46.7</v>
@@ -5009,7 +5009,7 @@
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1">
         <v>53.2</v>
@@ -5140,7 +5140,7 @@
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B37" s="1">
         <v>57.2</v>
@@ -5271,7 +5271,7 @@
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1">
         <v>64.099999999999994</v>
@@ -5402,7 +5402,7 @@
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1">
         <v>45.5</v>
@@ -5533,7 +5533,7 @@
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B40" s="1">
         <v>53.4</v>
@@ -5664,7 +5664,7 @@
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B41" s="1">
         <v>70.900000000000006</v>
@@ -5795,16 +5795,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="B1:AQ1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="V2:AA2"/>
+    <mergeCell ref="AB2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
@@ -5816,13 +5813,16 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
-    <mergeCell ref="B1:AQ1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="B2:U2"/>
-    <mergeCell ref="V2:AA2"/>
-    <mergeCell ref="AB2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>